<commit_message>
select and export excel from any
</commit_message>
<xml_diff>
--- a/db/excel/sqlite-inovation-manager-ver-5.0.xlsx
+++ b/db/excel/sqlite-inovation-manager-ver-5.0.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="546">
   <si>
     <t>table_name</t>
   </si>
@@ -1626,9 +1626,6 @@
     <t>trọng số là bao nhiêu</t>
   </si>
   <si>
-    <t>,   UNIQUE(idea_id, question_id, user_id), FOREIGN KEY (idea_id) REFERENCES ideas(id), , FOREIGN KEY (question_id) REFERENCES ideas_questions(id) , FOREIGN KEY (user_id) REFERENCES users(id)</t>
-  </si>
-  <si>
     <t>question</t>
   </si>
   <si>
@@ -1654,6 +1651,33 @@
   </si>
   <si>
     <t>Thứ tự sắp xếp (để người dùng xác định để dễ nhớ)</t>
+  </si>
+  <si>
+    <t>,   UNIQUE(idea_id, question_id, user_id), FOREIGN KEY (idea_id) REFERENCES ideas(id),  FOREIGN KEY (question_id) REFERENCES ideas_questions(id) , FOREIGN KEY (user_id) REFERENCES users(id)</t>
+  </si>
+  <si>
+    <t>Mã câu lệnh sql tạo ra</t>
+  </si>
+  <si>
+    <t>sql_logs</t>
+  </si>
+  <si>
+    <t>Mã user thực thi câu này</t>
+  </si>
+  <si>
+    <t>Thời gian tạo ra câu này</t>
+  </si>
+  <si>
+    <t>sql</t>
+  </si>
+  <si>
+    <t>Câu lệnh sql được lưu lại</t>
+  </si>
+  <si>
+    <t>0= select, 1=execute/run</t>
+  </si>
+  <si>
+    <t>Trạng thái để ghi thành công hay thất bại</t>
   </si>
 </sst>
 </file>
@@ -2090,9 +2114,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="182">
+  <cellStyleXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2625,7 +2651,7 @@
     <xf numFmtId="0" fontId="3" fillId="31" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="182">
+  <cellStyles count="184">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -2717,6 +2743,7 @@
     <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2807,6 +2834,7 @@
     <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3212,10 +3240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK241"/>
+  <dimension ref="A1:AMK247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="C234" sqref="C234"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="A242" sqref="A242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" x14ac:dyDescent="0"/>
@@ -7491,10 +7519,10 @@
         <v>21</v>
       </c>
       <c r="B169" s="146" t="s">
+        <v>533</v>
+      </c>
+      <c r="C169" s="99" t="s">
         <v>534</v>
-      </c>
-      <c r="C169" s="99" t="s">
-        <v>535</v>
       </c>
       <c r="D169" s="147" t="s">
         <v>519</v>
@@ -8595,7 +8623,7 @@
         <v>509</v>
       </c>
       <c r="B225" s="146" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C225" s="99" t="s">
         <v>511</v>
@@ -8750,7 +8778,7 @@
         <v>6</v>
       </c>
       <c r="C233" s="99" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D233" s="141" t="s">
         <v>439</v>
@@ -8769,7 +8797,7 @@
         <v>14</v>
       </c>
       <c r="C234" s="144" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D234" s="141" t="s">
         <v>439</v>
@@ -8910,11 +8938,131 @@
         <v>439</v>
       </c>
       <c r="E241" s="15" t="s">
-        <v>528</v>
+        <v>537</v>
       </c>
       <c r="F241" s="6"/>
       <c r="G241" s="6">
         <v>240</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7">
+      <c r="A242" s="107" t="s">
+        <v>539</v>
+      </c>
+      <c r="B242" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C242" s="92" t="s">
+        <v>538</v>
+      </c>
+      <c r="D242" s="130" t="s">
+        <v>439</v>
+      </c>
+      <c r="E242" s="17" t="s">
+        <v>450</v>
+      </c>
+      <c r="F242" s="6"/>
+      <c r="G242" s="6">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7">
+      <c r="A243" s="107" t="s">
+        <v>539</v>
+      </c>
+      <c r="B243" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="C243" s="92" t="s">
+        <v>540</v>
+      </c>
+      <c r="D243" s="130" t="s">
+        <v>439</v>
+      </c>
+      <c r="E243" s="6"/>
+      <c r="F243" s="6"/>
+      <c r="G243" s="6">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7">
+      <c r="A244" s="107" t="s">
+        <v>539</v>
+      </c>
+      <c r="B244" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="C244" s="92" t="s">
+        <v>541</v>
+      </c>
+      <c r="D244" s="130" t="s">
+        <v>439</v>
+      </c>
+      <c r="E244" s="6"/>
+      <c r="F244" s="6"/>
+      <c r="G244" s="6">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7">
+      <c r="A245" s="107" t="s">
+        <v>539</v>
+      </c>
+      <c r="B245" s="67" t="s">
+        <v>542</v>
+      </c>
+      <c r="C245" s="92" t="s">
+        <v>543</v>
+      </c>
+      <c r="D245" s="130" t="s">
+        <v>438</v>
+      </c>
+      <c r="E245" s="6"/>
+      <c r="F245" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G245" s="6">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7">
+      <c r="A246" s="107" t="s">
+        <v>539</v>
+      </c>
+      <c r="B246" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="C246" s="92" t="s">
+        <v>544</v>
+      </c>
+      <c r="D246" s="130" t="s">
+        <v>439</v>
+      </c>
+      <c r="E246" s="6"/>
+      <c r="F246" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G246" s="6">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7">
+      <c r="A247" s="107" t="s">
+        <v>539</v>
+      </c>
+      <c r="B247" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="C247" s="92" t="s">
+        <v>545</v>
+      </c>
+      <c r="D247" s="130" t="s">
+        <v>439</v>
+      </c>
+      <c r="E247" s="6"/>
+      <c r="F247" s="6"/>
+      <c r="G247" s="6">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -9820,7 +9968,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9843,7 +9991,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="146" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C1" s="146" t="s">
         <v>2</v>
@@ -9878,10 +10026,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -9898,10 +10046,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -9918,10 +10066,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D4">
         <v>0</v>

</xml_diff>